<commit_message>
Fix #14593 - [Bug] Fix nutrient export file for sugar
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportNutrients.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportNutrients.xlsx
@@ -15,10 +15,10 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">INCO!$A$3:$AL$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$J$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$M$3</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Produit!$B$3:$H$3</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">US!$A$3:$BA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$M$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutriments!$B$3:$T$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutriments!$B$3:$T$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutriments!$B$3:$T$3</definedName>
@@ -226,10 +226,10 @@
     <t xml:space="preserve">excel|IF(AE2="",IF(AD2="","",AD2),AE2)</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "Sucre"]_bcpg:nutListFormulatedValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "Sucre"]_bcpg:nutListValue</t>
+    <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "SUGAR"]_bcpg:nutListFormulatedValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "SUGAR"]_bcpg:nutListValue</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "SUGAD"]_bcpg:nutListFormulatedValue</t>
@@ -499,7 +499,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -540,6 +540,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="aakar"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -603,7 +609,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -662,6 +668,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -759,11 +769,11 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -855,11 +865,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -1034,7 +1044,7 @@
       <c r="AMJ3" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:J3"/>
+  <autoFilter ref="B3:M3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1051,62 +1061,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BO3"/>
+  <dimension ref="A1:BO7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ12" activeCellId="0" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="15" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="36" min="36" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="37" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="40" min="39" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="43" min="42" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="46" min="45" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="49" min="48" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="48" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="52" min="51" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="54" style="0" width="6.21"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1169,7 @@
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -1496,6 +1505,9 @@
         <v>127</v>
       </c>
       <c r="BB3" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:BA3"/>
@@ -1517,13 +1529,13 @@
   </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.06"/>
@@ -1531,37 +1543,37 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="36" min="36" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="37" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="911" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1611,7 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>

</xml_diff>